<commit_message>
Bug Fixes, Refactor admin.mjs, Responsive Fixes, Add numWeb SP, Add Vtas Adicionales Functionality
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\fullescabio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{345C5800-ECD6-4F0D-AB5D-B5AA88C4D225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8354F8BD-E446-4CDC-9547-31842780F26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A842995-D530-4971-9EF9-2E6B3D8272C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A842995-D530-4971-9EF9-2E6B3D8272C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,9 +547,6 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
       <c r="E6">
         <v>2</v>
       </c>
@@ -587,9 +584,6 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
       <c r="E8">
         <v>2</v>
       </c>
@@ -626,9 +620,6 @@
       </c>
       <c r="C10">
         <v>2</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
       </c>
       <c r="E10">
         <v>2</v>

</xml_diff>